<commit_message>
added final set of graphs
</commit_message>
<xml_diff>
--- a/figs/building-tag-CDFs.xlsx
+++ b/figs/building-tag-CDFs.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="soda" sheetId="1" r:id="rId1"/>
     <sheet name="sdh" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="campus wide" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="236">
   <si>
     <t xml:space="preserve"> site=SOD </t>
   </si>
@@ -723,6 +724,12 @@
   </si>
   <si>
     <t xml:space="preserve"> bypass valve=BYP.VLV </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chilled/condensor water loop-id </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hot water loop-id </t>
   </si>
 </sst>
 </file>
@@ -2319,11 +2326,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2068019784"/>
-        <c:axId val="-2068293720"/>
+        <c:axId val="2070412760"/>
+        <c:axId val="-2077830216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2068019784"/>
+        <c:axId val="2070412760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2353,12 +2360,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2068293720"/>
+        <c:crossAx val="-2077830216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2068293720"/>
+        <c:axId val="-2077830216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2410,7 +2417,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2068019784"/>
+        <c:crossAx val="2070412760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
@@ -3981,11 +3988,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2070548984"/>
-        <c:axId val="-2070522968"/>
+        <c:axId val="-2075992264"/>
+        <c:axId val="-2121379272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2070548984"/>
+        <c:axId val="-2075992264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3996,12 +4003,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2070522968"/>
+        <c:crossAx val="-2121379272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2070522968"/>
+        <c:axId val="-2121379272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -4014,7 +4021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2070548984"/>
+        <c:crossAx val="-2075992264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4888,11 +4895,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2070813880"/>
-        <c:axId val="-2070810856"/>
+        <c:axId val="-2070654296"/>
+        <c:axId val="-2075986184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2070813880"/>
+        <c:axId val="-2070654296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4902,12 +4909,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2070810856"/>
+        <c:crossAx val="-2075986184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2070810856"/>
+        <c:axId val="-2075986184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4918,14 +4925,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2070813880"/>
+        <c:crossAx val="-2070654296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5786,11 +5792,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2068055848"/>
-        <c:axId val="-2067894888"/>
+        <c:axId val="-2075757080"/>
+        <c:axId val="-2076094728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2068055848"/>
+        <c:axId val="-2075757080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5800,12 +5806,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067894888"/>
+        <c:crossAx val="-2076094728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2067894888"/>
+        <c:axId val="-2076094728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5816,7 +5822,1535 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2068055848"/>
+        <c:crossAx val="-2075757080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>% Points</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'campus wide'!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>79.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>97.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>102.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'campus wide'!$D$2:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>36.9096369096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.9096369096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.9966329966</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5807625808</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8594048594</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.48375648376</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.18755118755</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.18755118755</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.9103649104</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.9103649104</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2275002275</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.5217035217</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5217035217</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.01965601966</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.14905814906</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.30375830376</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.85385385385</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.12075712076</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.33415233415</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.33415233415</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.3215033215</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.21585221585</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.274001274</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.837200837201</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.54245154245</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.0637000637001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.914550914551</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.44235144235</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.764400764401</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.39585039585</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.25025025025</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.25025025025</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.40595140595</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.41505141505</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.3185003185</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.3114023114</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.40695240695</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.29065429065</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.750750750751</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.25025025025</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.778050778051</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.28765128765</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.655200655201</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.0849030849</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.4924014924</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.2184002184</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.40495040495</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.10465010465</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.02275002275</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.15015015015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2121735848"/>
+        <c:axId val="-2121732312"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>% Buildings</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'campus wide'!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>79.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>97.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>102.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'campus wide'!$E$2:$E$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>86.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>83.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>83.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>88.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>81.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>61.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>61.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>56.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>48.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>51.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>46.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>78.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>88.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>88.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>83.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>28.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>51.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>38.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>86.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>21.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>11.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>13.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>11.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>51.6666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2072528472"/>
+        <c:axId val="-2122293112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2121735848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2121732312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2121732312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="50.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2121735848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2122293112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2072528472"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2072528472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2122293112"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>% True Positive Points</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'campus wide'!$G$2:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>79.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>97.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>102.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'campus wide'!$I$2:$I$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.8028954708</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.6785079929</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.1735985533</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>73.2142857143</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77.2629310345</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.5139703346</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>81.0969299759</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>98.4962406015</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>93.26845093270001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>97.0839260313</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>91.0814606742</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>66.9365721997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21.4606021781</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.6209386282</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>86.6310160428</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>97.4137931034</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>92.3611111111</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>93.3333333333</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>97.7564102564</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>98.7261146497</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>23.6363636364</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>90.4605263158</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>90.522875817</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.400440044</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>77.63975155280001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>89.5683453237</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>48.3394833948</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>72.64573991029999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>% True Positive Buildings</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'campus wide'!$G$2:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>79.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>97.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>102.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'campus wide'!$J$2:$J$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55.5555555556</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.1428571429</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>93.87755102040001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>95.8333333333</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>87.2340425532</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>92.30769230769999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>48.4848484848</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>96.6666666667</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>97.82608695650001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>97.8723404255</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>55.5555555556</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>94.1176470588</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2029699624"/>
+        <c:axId val="-2029702072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2029699624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2029702072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2029702072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2029699624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5951,6 +7485,71 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1752600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6292,11 +7891,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1">
@@ -10471,7 +12073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
@@ -10482,4 +12084,1479 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>84.495641344999996</v>
+      </c>
+      <c r="D2">
+        <v>36.909636909600003</v>
+      </c>
+      <c r="E2">
+        <v>86.666666666699996</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3">
+        <v>84.495641344999996</v>
+      </c>
+      <c r="D3">
+        <v>36.909636909600003</v>
+      </c>
+      <c r="E3">
+        <v>86.666666666699996</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I3">
+        <v>95.802895470799996</v>
+      </c>
+      <c r="J3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4">
+        <v>72.540473225400007</v>
+      </c>
+      <c r="D4">
+        <v>32.996632996599999</v>
+      </c>
+      <c r="E4">
+        <v>61.666666666700003</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I4">
+        <v>26.678507992899998</v>
+      </c>
+      <c r="J4">
+        <v>55.555555555600002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>66.811955168099999</v>
+      </c>
+      <c r="D5">
+        <v>12.5807625808</v>
+      </c>
+      <c r="E5">
+        <v>58.333333333299997</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>68.173598553299996</v>
+      </c>
+      <c r="J5">
+        <v>97.142857142899999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>15.1307596513</v>
+      </c>
+      <c r="D6">
+        <v>4.8594048593999997</v>
+      </c>
+      <c r="E6">
+        <v>56.666666666700003</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>73.214285714300004</v>
+      </c>
+      <c r="J6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>14.4458281445</v>
+      </c>
+      <c r="D7">
+        <v>6.4837564837599997</v>
+      </c>
+      <c r="E7">
+        <v>66.666666666699996</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>77.262931034499999</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8">
+        <v>9.52677459527</v>
+      </c>
+      <c r="D8">
+        <v>1.18755118755</v>
+      </c>
+      <c r="E8">
+        <v>23.333333333300001</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
+      <c r="J8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>9.52677459527</v>
+      </c>
+      <c r="D9">
+        <v>1.18755118755</v>
+      </c>
+      <c r="E9">
+        <v>23.333333333300001</v>
+      </c>
+      <c r="G9">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>100</v>
+      </c>
+      <c r="J9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>6.6002490659999999</v>
+      </c>
+      <c r="D10">
+        <v>14.9103649104</v>
+      </c>
+      <c r="E10">
+        <v>83.333333333300004</v>
+      </c>
+      <c r="G10">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>90.513970334600003</v>
+      </c>
+      <c r="J10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11">
+        <v>6.4134495641299996</v>
+      </c>
+      <c r="D11">
+        <v>14.9103649104</v>
+      </c>
+      <c r="E11">
+        <v>83.333333333300004</v>
+      </c>
+      <c r="G11">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>170</v>
+      </c>
+      <c r="I11">
+        <v>81.096929975899997</v>
+      </c>
+      <c r="J11">
+        <v>93.877551020400006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>5.91531755915</v>
+      </c>
+      <c r="D12">
+        <v>0.22750022750000001</v>
+      </c>
+      <c r="E12">
+        <v>3.3333333333300001</v>
+      </c>
+      <c r="G12">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>3.9850560398499999</v>
+      </c>
+      <c r="D13">
+        <v>3.5217035217000001</v>
+      </c>
+      <c r="E13">
+        <v>65</v>
+      </c>
+      <c r="G13">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>100</v>
+      </c>
+      <c r="J13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14">
+        <v>3.4869240348699999</v>
+      </c>
+      <c r="D14">
+        <v>3.5217035217000001</v>
+      </c>
+      <c r="E14">
+        <v>65</v>
+      </c>
+      <c r="G14">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>145</v>
+      </c>
+      <c r="I14">
+        <v>98.496240601500006</v>
+      </c>
+      <c r="J14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>3.0510585305100002</v>
+      </c>
+      <c r="D15">
+        <v>6.0196560196600002</v>
+      </c>
+      <c r="E15">
+        <v>88.333333333300004</v>
+      </c>
+      <c r="G15">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <v>93.268450932700006</v>
+      </c>
+      <c r="J15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>1.9925280199299999</v>
+      </c>
+      <c r="D16">
+        <v>8.14905814906</v>
+      </c>
+      <c r="E16">
+        <v>80</v>
+      </c>
+      <c r="G16">
+        <v>22</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16">
+        <v>97.083926031299995</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17">
+        <v>1.9925280199299999</v>
+      </c>
+      <c r="D17">
+        <v>8.3037583037600005</v>
+      </c>
+      <c r="E17">
+        <v>81.666666666699996</v>
+      </c>
+      <c r="G17">
+        <v>23</v>
+      </c>
+      <c r="H17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I17">
+        <v>91.081460674200002</v>
+      </c>
+      <c r="J17">
+        <v>95.833333333300004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>1.9925280199299999</v>
+      </c>
+      <c r="D18">
+        <v>3.85385385385</v>
+      </c>
+      <c r="E18">
+        <v>80</v>
+      </c>
+      <c r="G18">
+        <v>24</v>
+      </c>
+      <c r="H18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18">
+        <v>66.936572199699995</v>
+      </c>
+      <c r="J18">
+        <v>87.234042553199998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>1.8679950186800001</v>
+      </c>
+      <c r="D19">
+        <v>7.1207571207599996</v>
+      </c>
+      <c r="E19">
+        <v>88.333333333300004</v>
+      </c>
+      <c r="G19">
+        <v>25</v>
+      </c>
+      <c r="H19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19">
+        <v>21.4606021781</v>
+      </c>
+      <c r="J19">
+        <v>92.307692307699995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>1.49439601494</v>
+      </c>
+      <c r="D20">
+        <v>2.3341523341500001</v>
+      </c>
+      <c r="E20">
+        <v>61.666666666700003</v>
+      </c>
+      <c r="G20">
+        <v>26</v>
+      </c>
+      <c r="H20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20">
+        <v>100</v>
+      </c>
+      <c r="J20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>235</v>
+      </c>
+      <c r="C21">
+        <v>1.49439601494</v>
+      </c>
+      <c r="D21">
+        <v>2.3341523341500001</v>
+      </c>
+      <c r="E21">
+        <v>61.666666666700003</v>
+      </c>
+      <c r="G21">
+        <v>27</v>
+      </c>
+      <c r="H21" t="s">
+        <v>235</v>
+      </c>
+      <c r="I21">
+        <v>100</v>
+      </c>
+      <c r="J21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>1.3698630137000001</v>
+      </c>
+      <c r="D22">
+        <v>3.3215033214999998</v>
+      </c>
+      <c r="E22">
+        <v>56.666666666700003</v>
+      </c>
+      <c r="G22">
+        <v>29</v>
+      </c>
+      <c r="H22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22">
+        <v>14.620938628199999</v>
+      </c>
+      <c r="J22">
+        <v>48.484848484799997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>1.1207970112100001</v>
+      </c>
+      <c r="D23">
+        <v>2.21585221585</v>
+      </c>
+      <c r="E23">
+        <v>48.333333333299997</v>
+      </c>
+      <c r="G23">
+        <v>31</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23">
+        <v>86.631016042799999</v>
+      </c>
+      <c r="J23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>0.80946450809500003</v>
+      </c>
+      <c r="D24">
+        <v>1.274001274</v>
+      </c>
+      <c r="E24">
+        <v>51.666666666700003</v>
+      </c>
+      <c r="G24">
+        <v>36</v>
+      </c>
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24">
+        <v>97.413793103399996</v>
+      </c>
+      <c r="J24">
+        <v>96.666666666699996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>0.74719800747200005</v>
+      </c>
+      <c r="D25">
+        <v>0.83720083720100003</v>
+      </c>
+      <c r="E25">
+        <v>46.666666666700003</v>
+      </c>
+      <c r="G25">
+        <v>37</v>
+      </c>
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25">
+        <v>92.361111111100001</v>
+      </c>
+      <c r="J25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>0.62266500622700005</v>
+      </c>
+      <c r="D26">
+        <v>1.54245154245</v>
+      </c>
+      <c r="E26">
+        <v>78.333333333300004</v>
+      </c>
+      <c r="G26">
+        <v>40</v>
+      </c>
+      <c r="H26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26">
+        <v>93.333333333300004</v>
+      </c>
+      <c r="J26">
+        <v>97.826086956500006</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>0.62266500622700005</v>
+      </c>
+      <c r="D27">
+        <v>6.3700063700099993E-2</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>41</v>
+      </c>
+      <c r="H27" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27">
+        <v>100</v>
+      </c>
+      <c r="J27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28">
+        <v>0.49813200498100002</v>
+      </c>
+      <c r="D28">
+        <v>0.91455091455100002</v>
+      </c>
+      <c r="E28">
+        <v>70</v>
+      </c>
+      <c r="G28">
+        <v>44</v>
+      </c>
+      <c r="H28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29">
+        <v>0.43586550435900001</v>
+      </c>
+      <c r="D29">
+        <v>1.4423514423499999</v>
+      </c>
+      <c r="E29">
+        <v>80</v>
+      </c>
+      <c r="G29">
+        <v>46</v>
+      </c>
+      <c r="H29" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29">
+        <v>97.756410256400002</v>
+      </c>
+      <c r="J29">
+        <v>97.872340425499999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>49</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30">
+        <v>0.37359900373600002</v>
+      </c>
+      <c r="D30">
+        <v>0.76440076440100002</v>
+      </c>
+      <c r="E30">
+        <v>45</v>
+      </c>
+      <c r="G30">
+        <v>49</v>
+      </c>
+      <c r="H30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30">
+        <v>98.726114649699994</v>
+      </c>
+      <c r="J30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>50</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31">
+        <v>0.37359900373600002</v>
+      </c>
+      <c r="D31">
+        <v>0.39585039584999998</v>
+      </c>
+      <c r="E31">
+        <v>15</v>
+      </c>
+      <c r="G31">
+        <v>50</v>
+      </c>
+      <c r="H31" t="s">
+        <v>38</v>
+      </c>
+      <c r="I31">
+        <v>100</v>
+      </c>
+      <c r="J31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32">
+        <v>0.37359900373600002</v>
+      </c>
+      <c r="D32">
+        <v>0.25025025024999997</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="G32">
+        <v>51</v>
+      </c>
+      <c r="H32" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32">
+        <v>100</v>
+      </c>
+      <c r="J32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33">
+        <v>0.31133250311299998</v>
+      </c>
+      <c r="D33">
+        <v>0.25025025024999997</v>
+      </c>
+      <c r="E33">
+        <v>15</v>
+      </c>
+      <c r="G33">
+        <v>52</v>
+      </c>
+      <c r="H33" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33">
+        <v>23.636363636399999</v>
+      </c>
+      <c r="J33">
+        <v>55.555555555600002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34">
+        <v>0.31133250311299998</v>
+      </c>
+      <c r="D34">
+        <v>1.40595140595</v>
+      </c>
+      <c r="E34">
+        <v>88.333333333300004</v>
+      </c>
+      <c r="G34">
+        <v>56</v>
+      </c>
+      <c r="H34" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34">
+        <v>90.460526315799996</v>
+      </c>
+      <c r="J34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35">
+        <v>0.31133250311299998</v>
+      </c>
+      <c r="D35">
+        <v>1.41505141505</v>
+      </c>
+      <c r="E35">
+        <v>88.333333333300004</v>
+      </c>
+      <c r="G35">
+        <v>58</v>
+      </c>
+      <c r="H35" t="s">
+        <v>46</v>
+      </c>
+      <c r="I35">
+        <v>90.522875816999999</v>
+      </c>
+      <c r="J35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36">
+        <v>0.31133250311299998</v>
+      </c>
+      <c r="D36">
+        <v>0.31850031849999999</v>
+      </c>
+      <c r="E36">
+        <v>65</v>
+      </c>
+      <c r="G36">
+        <v>59</v>
+      </c>
+      <c r="H36" t="s">
+        <v>47</v>
+      </c>
+      <c r="I36">
+        <v>100</v>
+      </c>
+      <c r="J36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37">
+        <v>62</v>
+      </c>
+      <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37">
+        <v>0.249066002491</v>
+      </c>
+      <c r="D37">
+        <v>2.3114023114000002</v>
+      </c>
+      <c r="E37">
+        <v>83.333333333300004</v>
+      </c>
+      <c r="G37">
+        <v>62</v>
+      </c>
+      <c r="H37" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38">
+        <v>66</v>
+      </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38">
+        <v>0.249066002491</v>
+      </c>
+      <c r="D38">
+        <v>2.4069524069499999</v>
+      </c>
+      <c r="E38">
+        <v>10</v>
+      </c>
+      <c r="G38">
+        <v>66</v>
+      </c>
+      <c r="H38" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38">
+        <v>100</v>
+      </c>
+      <c r="J38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
+        <v>181</v>
+      </c>
+      <c r="C39">
+        <v>0.249066002491</v>
+      </c>
+      <c r="D39">
+        <v>4.29065429065</v>
+      </c>
+      <c r="E39">
+        <v>28.333333333300001</v>
+      </c>
+      <c r="G39">
+        <v>70</v>
+      </c>
+      <c r="H39" t="s">
+        <v>181</v>
+      </c>
+      <c r="I39">
+        <v>4.4004400439999998</v>
+      </c>
+      <c r="J39">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40">
+        <v>71</v>
+      </c>
+      <c r="B40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40">
+        <v>0.249066002491</v>
+      </c>
+      <c r="D40">
+        <v>0.75075075075099995</v>
+      </c>
+      <c r="E40">
+        <v>51.666666666700003</v>
+      </c>
+      <c r="G40">
+        <v>71</v>
+      </c>
+      <c r="H40" t="s">
+        <v>57</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41">
+        <v>72</v>
+      </c>
+      <c r="B41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41">
+        <v>0.249066002491</v>
+      </c>
+      <c r="D41">
+        <v>0.25025025024999997</v>
+      </c>
+      <c r="E41">
+        <v>38.333333333299997</v>
+      </c>
+      <c r="G41">
+        <v>72</v>
+      </c>
+      <c r="H41" t="s">
+        <v>58</v>
+      </c>
+      <c r="I41">
+        <v>100</v>
+      </c>
+      <c r="J41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42">
+        <v>74</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42">
+        <v>0.249066002491</v>
+      </c>
+      <c r="D42">
+        <v>0.77805077805099998</v>
+      </c>
+      <c r="E42">
+        <v>65</v>
+      </c>
+      <c r="G42">
+        <v>74</v>
+      </c>
+      <c r="H42" t="s">
+        <v>60</v>
+      </c>
+      <c r="I42">
+        <v>77.639751552800007</v>
+      </c>
+      <c r="J42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43">
+        <v>75</v>
+      </c>
+      <c r="B43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43">
+        <v>0.249066002491</v>
+      </c>
+      <c r="D43">
+        <v>1.2876512876499999</v>
+      </c>
+      <c r="E43">
+        <v>86.666666666699996</v>
+      </c>
+      <c r="G43">
+        <v>75</v>
+      </c>
+      <c r="H43" t="s">
+        <v>61</v>
+      </c>
+      <c r="I43">
+        <v>89.568345323700001</v>
+      </c>
+      <c r="J43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44">
+        <v>0.249066002491</v>
+      </c>
+      <c r="D44">
+        <v>0.65520065520100002</v>
+      </c>
+      <c r="E44">
+        <v>21.666666666699999</v>
+      </c>
+      <c r="G44">
+        <v>77</v>
+      </c>
+      <c r="H44" t="s">
+        <v>63</v>
+      </c>
+      <c r="I44">
+        <v>80</v>
+      </c>
+      <c r="J44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45">
+        <v>79</v>
+      </c>
+      <c r="B45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45">
+        <v>0.249066002491</v>
+      </c>
+      <c r="D45">
+        <v>3.0849030849000001</v>
+      </c>
+      <c r="E45">
+        <v>11.666666666699999</v>
+      </c>
+      <c r="G45">
+        <v>79</v>
+      </c>
+      <c r="H45" t="s">
+        <v>65</v>
+      </c>
+      <c r="I45">
+        <v>48.339483394799998</v>
+      </c>
+      <c r="J45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46">
+        <v>85</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46">
+        <v>0.18679950186800001</v>
+      </c>
+      <c r="D46">
+        <v>1.4924014924</v>
+      </c>
+      <c r="E46">
+        <v>30</v>
+      </c>
+      <c r="G46">
+        <v>85</v>
+      </c>
+      <c r="H46" t="s">
+        <v>72</v>
+      </c>
+      <c r="I46">
+        <v>72.645739910299994</v>
+      </c>
+      <c r="J46">
+        <v>94.117647058800003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47">
+        <v>86</v>
+      </c>
+      <c r="B47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47">
+        <v>0.18679950186800001</v>
+      </c>
+      <c r="D47">
+        <v>0.21840021840000001</v>
+      </c>
+      <c r="E47">
+        <v>13.333333333300001</v>
+      </c>
+      <c r="G47">
+        <v>86</v>
+      </c>
+      <c r="H47" t="s">
+        <v>71</v>
+      </c>
+      <c r="I47">
+        <v>100</v>
+      </c>
+      <c r="J47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48">
+        <v>89</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48">
+        <v>0.124533001245</v>
+      </c>
+      <c r="D48">
+        <v>0.40495040495000001</v>
+      </c>
+      <c r="E48">
+        <v>80</v>
+      </c>
+      <c r="G48">
+        <v>89</v>
+      </c>
+      <c r="H48" t="s">
+        <v>75</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49">
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49">
+        <v>0.124533001245</v>
+      </c>
+      <c r="D49">
+        <v>0.10465010465000001</v>
+      </c>
+      <c r="E49">
+        <v>11.666666666699999</v>
+      </c>
+      <c r="G49">
+        <v>91</v>
+      </c>
+      <c r="H49" t="s">
+        <v>77</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50">
+        <v>97</v>
+      </c>
+      <c r="B50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50">
+        <v>0.124533001245</v>
+      </c>
+      <c r="D50">
+        <v>2.2750022750000001E-2</v>
+      </c>
+      <c r="E50">
+        <v>5</v>
+      </c>
+      <c r="G50">
+        <v>97</v>
+      </c>
+      <c r="H50" t="s">
+        <v>83</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51">
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51">
+        <v>6.2266500622699998E-2</v>
+      </c>
+      <c r="D51">
+        <v>0.15015015014999999</v>
+      </c>
+      <c r="E51">
+        <v>51.666666666700003</v>
+      </c>
+      <c r="G51">
+        <v>102</v>
+      </c>
+      <c r="H51" t="s">
+        <v>87</v>
+      </c>
+      <c r="I51">
+        <v>100</v>
+      </c>
+      <c r="J51">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>